<commit_message>
Corrected and Added Questions
Added questions around data classification and corrected question numbering.
</commit_message>
<xml_diff>
--- a/Environment Assessment.xlsx
+++ b/Environment Assessment.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mattfelton/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9533ABE-C810-4F47-862D-20A04847C441}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9D156963-20FB-DC43-8C2D-0734022568DE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" xr2:uid="{4D8EE577-1F65-8342-A339-968317300235}"/>
+    <workbookView xWindow="8400" yWindow="500" windowWidth="35840" windowHeight="20740" xr2:uid="{4D8EE577-1F65-8342-A339-968317300235}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="74">
   <si>
     <t>Question</t>
   </si>
@@ -235,9 +235,6 @@
     <t>If Azure is already in use, what is the network design that is being used (hub and spoke, VWAN, etc)?</t>
   </si>
   <si>
-    <t>If Azure is already in use, what aregions are being used?</t>
-  </si>
-  <si>
     <t>If Azure is already in use, how is logging being handled?</t>
   </si>
   <si>
@@ -251,6 +248,15 @@
   </si>
   <si>
     <t>Microsoft Comments</t>
+  </si>
+  <si>
+    <t>Is the organization using containers? If so, what container runtime is the organization using? What about container management?</t>
+  </si>
+  <si>
+    <t>Does the organization have a formal data classification system? Is there a documented set of controls applicable to each data classification? Are workloads classified using this system?</t>
+  </si>
+  <si>
+    <t>If Azure is already in use, what regions are being used?</t>
   </si>
 </sst>
 </file>
@@ -282,7 +288,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -292,6 +298,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF0070C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -308,7 +320,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -325,35 +337,22 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="7">
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment vertical="bottom" textRotation="0" wrapText="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="bottom" textRotation="0" wrapText="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -415,6 +414,31 @@
       </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -429,15 +453,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{0A150142-D5DA-F248-BB3A-DB4DC473B2F3}" name="Table4" displayName="Table4" ref="A1:F59" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="A1:F59" xr:uid="{31923BB3-17AC-8A46-942E-8A8A248580F9}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{0A150142-D5DA-F248-BB3A-DB4DC473B2F3}" name="Table4" displayName="Table4" ref="A1:F61" totalsRowShown="0" headerRowDxfId="6">
+  <autoFilter ref="A1:F61" xr:uid="{31923BB3-17AC-8A46-942E-8A8A248580F9}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{342B37FF-A3C7-BB46-BF74-222EFF2CEFBA}" name="Domain" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{FC3B8143-8695-B941-8639-2A077A76ACD7}" name="#" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{E62E4B4B-6E98-2549-8490-AD6649BD3CEC}" name="Azure" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{411D171C-5D13-8844-A6DE-B8FB05305653}" name="Question" dataDxfId="1"/>
-    <tableColumn id="5" xr3:uid="{734EC95D-7AD3-C64D-ADA7-36504E4D6188}" name="Customer Response"/>
-    <tableColumn id="6" xr3:uid="{B6091B8E-CC64-6141-8DA1-39CAED4CE723}" name="Microsoft Comments"/>
+    <tableColumn id="1" xr3:uid="{342B37FF-A3C7-BB46-BF74-222EFF2CEFBA}" name="Domain" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{FC3B8143-8695-B941-8639-2A077A76ACD7}" name="#" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{E62E4B4B-6E98-2549-8490-AD6649BD3CEC}" name="Azure" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{411D171C-5D13-8844-A6DE-B8FB05305653}" name="Question" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{734EC95D-7AD3-C64D-ADA7-36504E4D6188}" name="Customer Response" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{B6091B8E-CC64-6141-8DA1-39CAED4CE723}" name="Microsoft Comments" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -740,10 +764,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40364CCC-36A0-7340-82AA-5C98C2F20104}">
-  <dimension ref="A1:F59"/>
+  <dimension ref="A1:F61"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="117" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A35" zoomScale="117" workbookViewId="0">
+      <selection activeCell="E45" sqref="E45:F61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -752,8 +776,8 @@
     <col min="2" max="2" width="6.1640625" style="1" customWidth="1"/>
     <col min="3" max="3" width="10.5" style="1" customWidth="1"/>
     <col min="4" max="4" width="54.6640625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="33.83203125" customWidth="1"/>
-    <col min="6" max="6" width="27.1640625" customWidth="1"/>
+    <col min="5" max="5" width="33.83203125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="27.1640625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" ht="20" x14ac:dyDescent="0.25">
@@ -769,11 +793,11 @@
       <c r="D1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="4" t="s">
-        <v>71</v>
+      <c r="F1" s="5" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -956,7 +980,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>17</v>
       </c>
@@ -970,7 +994,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>17</v>
       </c>
@@ -984,7 +1008,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>21</v>
       </c>
@@ -996,7 +1020,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>21</v>
       </c>
@@ -1008,7 +1032,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>21</v>
       </c>
@@ -1019,8 +1043,9 @@
       <c r="D21" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="E21" s="6"/>
+    </row>
+    <row r="22" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>21</v>
       </c>
@@ -1029,10 +1054,11 @@
       </c>
       <c r="C22" s="3"/>
       <c r="D22" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+        <v>71</v>
+      </c>
+      <c r="F22" s="7"/>
+    </row>
+    <row r="23" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>21</v>
       </c>
@@ -1041,10 +1067,11 @@
       </c>
       <c r="C23" s="3"/>
       <c r="D23" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+        <v>26</v>
+      </c>
+      <c r="E23" s="7"/>
+    </row>
+    <row r="24" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>21</v>
       </c>
@@ -1053,10 +1080,10 @@
       </c>
       <c r="C24" s="3"/>
       <c r="D24" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>21</v>
       </c>
@@ -1065,10 +1092,10 @@
       </c>
       <c r="C25" s="3"/>
       <c r="D25" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>21</v>
       </c>
@@ -1077,10 +1104,10 @@
       </c>
       <c r="C26" s="3"/>
       <c r="D26" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>21</v>
       </c>
@@ -1089,81 +1116,80 @@
       </c>
       <c r="C27" s="3"/>
       <c r="D27" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>21</v>
       </c>
       <c r="B28" s="3">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C28" s="3"/>
       <c r="D28" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>21</v>
       </c>
       <c r="B29" s="3">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C29" s="3"/>
       <c r="D29" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
         <v>21</v>
       </c>
       <c r="B30" s="3">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C30" s="3"/>
       <c r="D30" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
         <v>21</v>
       </c>
       <c r="B31" s="3">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C31" s="3"/>
       <c r="D31" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+        <v>55</v>
+      </c>
+      <c r="E31" s="6"/>
+    </row>
+    <row r="32" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
         <v>21</v>
       </c>
       <c r="B32" s="3">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C32" s="3"/>
       <c r="D32" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A33" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B33" s="3">
+        <v>15</v>
+      </c>
+      <c r="C33" s="3"/>
+      <c r="D33" s="2" t="s">
         <v>57</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A33" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B33" s="3">
-        <v>13</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1171,99 +1197,101 @@
         <v>21</v>
       </c>
       <c r="B34" s="3">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C34" s="3" t="s">
         <v>63</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
         <v>21</v>
       </c>
       <c r="B35" s="3">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C35" s="3" t="s">
         <v>63</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="B36" s="3">
-        <v>1</v>
-      </c>
-      <c r="C36" s="3"/>
+        <v>18</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>63</v>
+      </c>
       <c r="D36" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B37" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C37" s="3"/>
       <c r="D37" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B38" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C38" s="3"/>
       <c r="D38" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B39" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C39" s="3"/>
       <c r="D39" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B40" s="3">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C40" s="3"/>
       <c r="D40" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B41" s="3">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C41" s="3"/>
       <c r="D41" s="2" t="s">
-        <v>53</v>
+        <v>29</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -1271,77 +1299,77 @@
         <v>14</v>
       </c>
       <c r="B42" s="3">
-        <v>7</v>
-      </c>
-      <c r="C42" s="3" t="s">
-        <v>63</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="C42" s="3"/>
       <c r="D42" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B43" s="3">
-        <v>8</v>
-      </c>
-      <c r="C43" s="3" t="s">
-        <v>63</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="C43" s="3"/>
       <c r="D43" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B44" s="3">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C44" s="3" t="s">
         <v>63</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
-        <v>33</v>
+        <v>14</v>
       </c>
       <c r="B45" s="3">
-        <v>1</v>
-      </c>
-      <c r="C45" s="3"/>
+        <v>9</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>63</v>
+      </c>
       <c r="D45" s="2" t="s">
-        <v>35</v>
+        <v>60</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
-        <v>33</v>
+        <v>14</v>
       </c>
       <c r="B46" s="3">
-        <v>2</v>
-      </c>
-      <c r="C46" s="3"/>
+        <v>10</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>63</v>
+      </c>
       <c r="D46" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="59" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
         <v>33</v>
       </c>
       <c r="B47" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C47" s="3"/>
       <c r="D47" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="51" x14ac:dyDescent="0.2">
@@ -1349,83 +1377,83 @@
         <v>33</v>
       </c>
       <c r="B48" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C48" s="3"/>
       <c r="D48" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
         <v>33</v>
       </c>
       <c r="B49" s="3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C49" s="3"/>
       <c r="D49" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
         <v>33</v>
       </c>
       <c r="B50" s="3">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C50" s="3"/>
       <c r="D50" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
         <v>33</v>
       </c>
       <c r="B51" s="3">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C51" s="3"/>
       <c r="D51" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" ht="102" x14ac:dyDescent="0.2">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
         <v>33</v>
       </c>
       <c r="B52" s="3">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C52" s="3"/>
       <c r="D52" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="B53" s="3">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C53" s="3"/>
       <c r="D53" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="102" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="B54" s="3">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C54" s="3"/>
       <c r="D54" s="2" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -1433,25 +1461,23 @@
         <v>46</v>
       </c>
       <c r="B55" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C55" s="3"/>
       <c r="D55" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A56" s="3" t="s">
         <v>46</v>
       </c>
       <c r="B56" s="3">
-        <v>4</v>
-      </c>
-      <c r="C56" s="3" t="s">
-        <v>63</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="C56" s="3"/>
       <c r="D56" s="2" t="s">
-        <v>69</v>
+        <v>48</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -1459,43 +1485,69 @@
         <v>46</v>
       </c>
       <c r="B57" s="3">
-        <v>5</v>
-      </c>
-      <c r="C57" s="3" t="s">
-        <v>63</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="C57" s="3"/>
       <c r="D57" s="2" t="s">
-        <v>70</v>
+        <v>49</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A58" s="3" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B58" s="3">
-        <v>1</v>
-      </c>
-      <c r="C58" s="3"/>
+        <v>4</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>63</v>
+      </c>
       <c r="D58" s="2" t="s">
-        <v>52</v>
+        <v>68</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A59" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B59" s="3">
+        <v>5</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A60" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B59" s="3">
+      <c r="B60" s="3">
+        <v>1</v>
+      </c>
+      <c r="C60" s="3"/>
+      <c r="D60" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A61" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B61" s="3">
         <v>2</v>
       </c>
-      <c r="C59" s="3"/>
-      <c r="D59" s="2" t="s">
+      <c r="C61" s="3"/>
+      <c r="D61" s="2" t="s">
         <v>51</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A53:D59">
-    <sortCondition ref="A53:A59"/>
-    <sortCondition ref="B53:B59"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A55:D61">
+    <sortCondition ref="A55:A61"/>
+    <sortCondition ref="B55:B61"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>